<commit_message>
clear code by chat gtp
</commit_message>
<xml_diff>
--- a/bin/config/xlsx/Ability.xlsx
+++ b/bin/config/xlsx/Ability.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17200"/>
+    <workbookView windowWidth="28800" windowHeight="12255"/>
   </bookViews>
   <sheets>
     <sheet name="Ability" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="41">
   <si>
     <t>id</t>
   </si>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t>postcastrecoverytime</t>
-  </si>
-  <si>
-    <t>channelstart</t>
   </si>
   <si>
     <t>channelthink</t>
@@ -851,7 +848,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="CCE8CF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1101,15 +1098,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AL21"/>
+  <dimension ref="A1:AK21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AF1" sqref="AF1"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData>
-    <row r="1" spans="1:38">
+    <row r="1" spans="1:37">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1186,19 +1183,19 @@
         <v>15</v>
       </c>
       <c r="Z1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="AA1" t="s">
         <v>15</v>
       </c>
       <c r="AB1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="AC1" t="s">
         <v>15</v>
       </c>
       <c r="AD1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="AE1" t="s">
         <v>15</v>
@@ -1221,298 +1218,292 @@
       <c r="AK1" t="s">
         <v>21</v>
       </c>
-      <c r="AL1" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="2" spans="1:38">
+    <row r="2" spans="1:37">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="W2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="X2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Y2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Z2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AA2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AB2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AC2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AD2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AE2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AF2" t="s">
         <v>23</v>
       </c>
       <c r="AG2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AH2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AI2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="AJ2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AK2" t="s">
-        <v>23</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:38">
+    <row r="4" spans="1:37">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="S4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="T4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="U4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="V4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="W4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="X4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Y4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Z4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AA4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AB4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AC4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AD4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AE4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AF4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AG4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AH4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AI4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AJ4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AK4" t="s">
-        <v>25</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="6:6">
       <c r="F5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" ht="409.5" spans="2:37">
+      <c r="B7" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" ht="409.5" spans="2:38">
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="F7" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>29</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" t="s">
         <v>31</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>32</v>
       </c>
-      <c r="J7" t="s">
+      <c r="S7" t="s">
         <v>33</v>
       </c>
-      <c r="S7" t="s">
+      <c r="X7" t="s">
         <v>34</v>
       </c>
       <c r="Y7" t="s">
         <v>35</v>
       </c>
       <c r="Z7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AA7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AB7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="AC7" t="s">
         <v>35</v>
       </c>
       <c r="AD7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AE7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AF7" t="s">
         <v>36</v>
@@ -1530,10 +1521,7 @@
         <v>40</v>
       </c>
       <c r="AK7" t="s">
-        <v>41</v>
-      </c>
-      <c r="AL7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="2:5">
@@ -1548,7 +1536,7 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:38">
+    <row r="10" spans="1:37">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1610,7 +1598,7 @@
         <v>1</v>
       </c>
       <c r="V10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W10">
         <v>0</v>
@@ -1657,11 +1645,8 @@
       <c r="AK10">
         <v>0</v>
       </c>
-      <c r="AL10">
-        <v>0</v>
-      </c>
     </row>
-    <row r="11" spans="1:38">
+    <row r="11" spans="1:37">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1723,7 +1708,7 @@
         <v>1</v>
       </c>
       <c r="V11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W11">
         <v>0</v>
@@ -1770,11 +1755,8 @@
       <c r="AK11">
         <v>0</v>
       </c>
-      <c r="AL11">
-        <v>0</v>
-      </c>
     </row>
-    <row r="12" spans="1:38">
+    <row r="12" spans="1:37">
       <c r="A12">
         <v>3</v>
       </c>
@@ -1836,7 +1818,7 @@
         <v>1</v>
       </c>
       <c r="V12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W12">
         <v>0</v>
@@ -1883,11 +1865,8 @@
       <c r="AK12">
         <v>0</v>
       </c>
-      <c r="AL12">
-        <v>0</v>
-      </c>
     </row>
-    <row r="13" spans="1:38">
+    <row r="13" spans="1:37">
       <c r="A13">
         <v>4</v>
       </c>
@@ -1949,7 +1928,7 @@
         <v>1</v>
       </c>
       <c r="V13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W13">
         <v>0</v>
@@ -1996,11 +1975,8 @@
       <c r="AK13">
         <v>0</v>
       </c>
-      <c r="AL13">
-        <v>0</v>
-      </c>
     </row>
-    <row r="14" spans="1:38">
+    <row r="14" spans="1:37">
       <c r="A14">
         <v>5</v>
       </c>
@@ -2062,7 +2038,7 @@
         <v>1</v>
       </c>
       <c r="V14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W14">
         <v>0</v>
@@ -2109,11 +2085,8 @@
       <c r="AK14">
         <v>0</v>
       </c>
-      <c r="AL14">
-        <v>0</v>
-      </c>
     </row>
-    <row r="15" spans="1:38">
+    <row r="15" spans="1:37">
       <c r="A15">
         <v>6</v>
       </c>
@@ -2178,7 +2151,7 @@
         <v>1</v>
       </c>
       <c r="V15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W15">
         <v>0</v>
@@ -2225,11 +2198,8 @@
       <c r="AK15">
         <v>0</v>
       </c>
-      <c r="AL15">
-        <v>0</v>
-      </c>
     </row>
-    <row r="16" spans="1:38">
+    <row r="16" spans="1:37">
       <c r="A16">
         <v>7</v>
       </c>
@@ -2291,7 +2261,7 @@
         <v>1</v>
       </c>
       <c r="V16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W16">
         <v>0</v>
@@ -2338,11 +2308,8 @@
       <c r="AK16">
         <v>0</v>
       </c>
-      <c r="AL16">
-        <v>0</v>
-      </c>
     </row>
-    <row r="17" spans="1:38">
+    <row r="17" spans="1:37">
       <c r="A17">
         <v>8</v>
       </c>
@@ -2404,7 +2371,7 @@
         <v>1</v>
       </c>
       <c r="V17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W17">
         <v>0</v>
@@ -2451,11 +2418,8 @@
       <c r="AK17">
         <v>0</v>
       </c>
-      <c r="AL17">
-        <v>0</v>
-      </c>
     </row>
-    <row r="18" spans="1:38">
+    <row r="18" spans="1:37">
       <c r="A18">
         <v>9</v>
       </c>
@@ -2517,7 +2481,7 @@
         <v>1</v>
       </c>
       <c r="V18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W18">
         <v>0</v>
@@ -2564,11 +2528,8 @@
       <c r="AK18">
         <v>0</v>
       </c>
-      <c r="AL18">
-        <v>0</v>
-      </c>
     </row>
-    <row r="19" spans="1:38">
+    <row r="19" spans="1:37">
       <c r="A19">
         <v>10</v>
       </c>
@@ -2630,7 +2591,7 @@
         <v>1</v>
       </c>
       <c r="V19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W19">
         <v>0</v>
@@ -2677,11 +2638,8 @@
       <c r="AK19">
         <v>0</v>
       </c>
-      <c r="AL19">
-        <v>0</v>
-      </c>
     </row>
-    <row r="20" spans="1:38">
+    <row r="20" spans="1:37">
       <c r="A20">
         <v>11</v>
       </c>
@@ -2743,7 +2701,7 @@
         <v>1</v>
       </c>
       <c r="V20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W20">
         <v>0</v>
@@ -2790,11 +2748,8 @@
       <c r="AK20">
         <v>0</v>
       </c>
-      <c r="AL20">
-        <v>0</v>
-      </c>
     </row>
-    <row r="21" spans="1:38">
+    <row r="21" spans="1:37">
       <c r="A21">
         <v>12</v>
       </c>
@@ -2859,7 +2814,7 @@
         <v>1</v>
       </c>
       <c r="V21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W21">
         <v>0</v>
@@ -2904,9 +2859,6 @@
         <v>0</v>
       </c>
       <c r="AK21">
-        <v>0</v>
-      </c>
-      <c r="AL21">
         <v>0</v>
       </c>
     </row>

</xml_diff>